<commit_message>
TST: add test cases for date comparison. Fixes #268
</commit_message>
<xml_diff>
--- a/tests/sales.xlsx
+++ b/tests/sales.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sales" sheetId="1" r:id="rId1"/>
-    <sheet name="dummy" sheetId="2" r:id="rId2"/>
+    <sheet name="dates" sheetId="3" r:id="rId2"/>
+    <sheet name="dummy" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="19">
   <si>
     <t>product</t>
   </si>
@@ -79,6 +80,9 @@
   </si>
   <si>
     <t>This is a help sheet</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -88,7 +92,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +101,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,12 +137,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -879,6 +893,359 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>43101</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <f>A2+1</f>
+        <v>43102</v>
+      </c>
+      <c r="B3">
+        <f>B2+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A34" si="0">A3+1</f>
+        <v>43103</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B34" si="1">B3+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>43104</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>43105</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>43106</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>43107</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>43108</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>43109</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>43110</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>43111</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <f t="shared" si="0"/>
+        <v>43112</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f t="shared" si="0"/>
+        <v>43113</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <f t="shared" si="0"/>
+        <v>43114</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f t="shared" si="0"/>
+        <v>43115</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <f t="shared" si="0"/>
+        <v>43116</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <f t="shared" si="0"/>
+        <v>43117</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f t="shared" si="0"/>
+        <v>43118</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <f t="shared" si="0"/>
+        <v>43119</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f t="shared" si="0"/>
+        <v>43120</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f t="shared" si="0"/>
+        <v>43121</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <f t="shared" si="0"/>
+        <v>43122</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f t="shared" si="0"/>
+        <v>43123</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <f t="shared" si="0"/>
+        <v>43124</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <f t="shared" si="0"/>
+        <v>43125</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <f t="shared" si="0"/>
+        <v>43126</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <f t="shared" si="0"/>
+        <v>43127</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <f t="shared" si="0"/>
+        <v>43128</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <f t="shared" si="0"/>
+        <v>43129</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <f t="shared" si="0"/>
+        <v>43130</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <f t="shared" si="0"/>
+        <v>43131</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <f t="shared" si="0"/>
+        <v>43132</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <f t="shared" si="0"/>
+        <v>43133</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
BUG: FormHandler should pass table= to Excel reader
</commit_message>
<xml_diff>
--- a/tests/sales.xlsx
+++ b/tests/sales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\site\gramener.com\viz\async-gramex\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948605C7-75F2-4DE7-A076-8D7742DEEC9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B960B43A-7FA7-4EEC-906F-DBE12E69798F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6EE3D399-FAD5-3F44-9EB5-0B167948DCE0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6EE3D399-FAD5-3F44-9EB5-0B167948DCE0}"/>
   </bookViews>
   <sheets>
     <sheet name="sales" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="1317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="1317">
   <si>
     <t>देश</t>
   </si>
@@ -4115,6 +4115,20 @@
     <tableColumn id="1" xr3:uid="{A5F73EF8-4814-419F-8434-EF234D1DE6CC}" name="State"/>
     <tableColumn id="2" xr3:uid="{7F6E1914-BFE5-4E80-BE05-DD65E9A997D1}" name="District"/>
     <tableColumn id="3" xr3:uid="{A74C1237-C79F-42E2-B108-485614EAF929}" name="DistrictCaps"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D997A2B0-9478-46AF-8A22-AF84E153EAE3}" name="MainTable" displayName="MainTable" ref="H1:L25" totalsRowShown="0">
+  <autoFilter ref="H1:L25" xr:uid="{2BBE5A03-AA86-49B4-8A30-3A3BBB0BD567}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{456B5CDA-DAA2-41C9-B7AA-AF5D6422D118}" name="देश"/>
+    <tableColumn id="2" xr3:uid="{48F64B5B-1A57-48CA-85CA-22B386CC0DEA}" name="city"/>
+    <tableColumn id="3" xr3:uid="{1B83E8C8-E8B0-4F35-8A50-11051B4A6863}" name="product"/>
+    <tableColumn id="4" xr3:uid="{DECD69B3-74B4-4822-886E-647BC83DE5FD}" name="sales"/>
+    <tableColumn id="5" xr3:uid="{E619E771-82DD-44E5-8E67-0AF40B87A994}" name="growth"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4419,7 +4433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5832FD-D67F-1D4C-95D0-0EB623A26DB3}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12208,17 +12224,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659752B2-EC32-4E9A-A211-175F3CF07DC6}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.75" customWidth="1"/>
+    <col min="10" max="10" width="9.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -12234,8 +12251,23 @@
       <c r="F1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -12251,8 +12283,23 @@
       <c r="F2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <v>866.1</v>
+      </c>
+      <c r="L2">
+        <v>-0.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43102</v>
       </c>
@@ -12268,8 +12315,23 @@
       <c r="F3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>26.4</v>
+      </c>
+      <c r="L3">
+        <v>-0.24199999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43103</v>
       </c>
@@ -12285,8 +12347,23 @@
       <c r="F4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="L4">
+        <v>-0.29099999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43104</v>
       </c>
@@ -12302,8 +12379,23 @@
       <c r="F5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>513.70000000000005</v>
+      </c>
+      <c r="L5">
+        <v>-0.113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43105</v>
       </c>
@@ -12319,8 +12411,23 @@
       <c r="F6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>41.9</v>
+      </c>
+      <c r="L6">
+        <v>-0.40200000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43106</v>
       </c>
@@ -12336,8 +12443,23 @@
       <c r="F7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>52.2</v>
+      </c>
+      <c r="L7">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43107</v>
       </c>
@@ -12353,8 +12475,23 @@
       <c r="F8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <v>17.8</v>
+      </c>
+      <c r="L8">
+        <v>-5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43108</v>
       </c>
@@ -12370,8 +12507,23 @@
       <c r="F9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>178.9</v>
+      </c>
+      <c r="L9">
+        <v>-0.26100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43109</v>
       </c>
@@ -12387,8 +12539,23 @@
       <c r="F10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10">
+        <v>217.4</v>
+      </c>
+      <c r="L10">
+        <v>0.114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43110</v>
       </c>
@@ -12404,8 +12571,17 @@
       <c r="F11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>21</v>
       </c>
@@ -12415,8 +12591,23 @@
       <c r="F12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12">
+        <v>94.4</v>
+      </c>
+      <c r="L12">
+        <v>-0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>21</v>
       </c>
@@ -12426,8 +12617,23 @@
       <c r="F13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <v>72.8</v>
+      </c>
+      <c r="L13">
+        <v>-6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>21</v>
       </c>
@@ -12437,8 +12643,23 @@
       <c r="F14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14">
+        <v>671</v>
+      </c>
+      <c r="L14">
+        <v>-1.4E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>21</v>
       </c>
@@ -12448,8 +12669,23 @@
       <c r="F15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15">
+        <v>560.20000000000005</v>
+      </c>
+      <c r="L15">
+        <v>-0.19700000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>21</v>
       </c>
@@ -12459,8 +12695,23 @@
       <c r="F16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16">
+        <v>237.9</v>
+      </c>
+      <c r="L16">
+        <v>0.19400000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>21</v>
       </c>
@@ -12470,8 +12721,23 @@
       <c r="F17" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <v>719</v>
+      </c>
+      <c r="L17">
+        <v>0.11799999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>21</v>
       </c>
@@ -12481,8 +12747,23 @@
       <c r="F18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18">
+        <v>18.3</v>
+      </c>
+      <c r="L18">
+        <v>-0.154</v>
+      </c>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>21</v>
       </c>
@@ -12492,8 +12773,23 @@
       <c r="F19" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>41.6</v>
+      </c>
+      <c r="L19">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>21</v>
       </c>
@@ -12503,8 +12799,23 @@
       <c r="F20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20">
+        <v>32.4</v>
+      </c>
+      <c r="L20">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>21</v>
       </c>
@@ -12514,8 +12825,23 @@
       <c r="F21" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <v>12.5</v>
+      </c>
+      <c r="L21">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>21</v>
       </c>
@@ -12525,8 +12851,23 @@
       <c r="F22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22">
+        <v>1352.4</v>
+      </c>
+      <c r="L22">
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>21</v>
       </c>
@@ -12536,12 +12877,56 @@
       <c r="F23" t="s">
         <v>65</v>
       </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23">
+        <v>190.2</v>
+      </c>
+      <c r="L23">
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24">
+        <v>148.19999999999999</v>
+      </c>
+      <c r="L24">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
TST: Add a sample test case. Fix typo in data.py
</commit_message>
<xml_diff>
--- a/tests/sales.xlsx
+++ b/tests/sales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\site\gramener.com\viz\async-gramex\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\site\gramener.com\viz\async-gramex\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B960B43A-7FA7-4EEC-906F-DBE12E69798F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A18EA7-C0C5-42F0-83D7-9D4E1BF929EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6EE3D399-FAD5-3F44-9EB5-0B167948DCE0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6EE3D399-FAD5-3F44-9EB5-0B167948DCE0}"/>
   </bookViews>
   <sheets>
     <sheet name="sales" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="census" sheetId="3" r:id="rId3"/>
     <sheet name="table" sheetId="5" r:id="rId4"/>
     <sheet name="dummy" sheetId="4" r:id="rId5"/>
+    <sheet name="cities" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="census" localSheetId="2">census!$A$1:$C$641</definedName>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="1317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="1321">
   <si>
     <t>देश</t>
   </si>
@@ -4026,6 +4027,18 @@
   </si>
   <si>
     <t>This is a help sheet</t>
+  </si>
+  <si>
+    <t>drive</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>demand</t>
   </si>
 </sst>
 </file>
@@ -4433,9 +4446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5832FD-D67F-1D4C-95D0-0EB623A26DB3}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12226,7 +12237,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659752B2-EC32-4E9A-A211-175F3CF07DC6}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12947,4 +12960,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{933B7139-EFBD-4D13-AF10-856D11616FDD}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C7">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ENH: gramex.cache.open(excel) supports hyperlinks. Fixes #722
</commit_message>
<xml_diff>
--- a/tests/sales.xlsx
+++ b/tests/sales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\site\gramener.com\viz\async-gramex\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\site\gramener.com\viz\async-gramex\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B960B43A-7FA7-4EEC-906F-DBE12E69798F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4BAC76-22CE-477D-BACB-5FB8165625D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6EE3D399-FAD5-3F44-9EB5-0B167948DCE0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{6EE3D399-FAD5-3F44-9EB5-0B167948DCE0}"/>
   </bookViews>
   <sheets>
     <sheet name="sales" sheetId="1" r:id="rId1"/>
@@ -4032,10 +4032,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4058,14 +4066,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -4433,9 +4444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5832FD-D67F-1D4C-95D0-0EB623A26DB3}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12277,13 +12286,13 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I2" t="s">
@@ -12309,13 +12318,13 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I3" t="s">
@@ -12341,13 +12350,13 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I4" t="s">
@@ -12373,13 +12382,13 @@
       <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I5" t="s">
@@ -12405,13 +12414,13 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I6" t="s">
@@ -12437,13 +12446,13 @@
       <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I7" t="s">
@@ -12469,13 +12478,13 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I8" t="s">
@@ -12501,13 +12510,13 @@
       <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F9" t="s">
         <v>37</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I9" t="s">
@@ -12533,13 +12542,13 @@
       <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I10" t="s">
@@ -12565,13 +12574,13 @@
       <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I11" t="s">
@@ -12585,13 +12594,13 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F12" t="s">
         <v>43</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I12" t="s">
@@ -12611,13 +12620,13 @@
       <c r="D13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F13" t="s">
         <v>45</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I13" t="s">
@@ -12637,13 +12646,13 @@
       <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F14" t="s">
         <v>47</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I14" t="s">
@@ -12663,13 +12672,13 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F15" t="s">
         <v>49</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I15" t="s">
@@ -12689,13 +12698,13 @@
       <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F16" t="s">
         <v>51</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I16" t="s">
@@ -12715,13 +12724,13 @@
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F17" t="s">
         <v>53</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I17" t="s">
@@ -12741,13 +12750,13 @@
       <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F18" t="s">
         <v>55</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I18" t="s">
@@ -12767,13 +12776,13 @@
       <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F19" t="s">
         <v>57</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I19" t="s">
@@ -12793,13 +12802,13 @@
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F20" t="s">
         <v>59</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I20" t="s">
@@ -12819,13 +12828,13 @@
       <c r="D21" t="s">
         <v>21</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F21" t="s">
         <v>61</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I21" t="s">
@@ -12845,13 +12854,13 @@
       <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F22" t="s">
         <v>63</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I22" t="s">
@@ -12871,13 +12880,13 @@
       <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F23" t="s">
         <v>65</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I23" t="s">
@@ -12894,7 +12903,7 @@
       </c>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H24" t="s">
+      <c r="H24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I24" t="s">
@@ -12911,7 +12920,7 @@
       </c>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
+      <c r="H25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I25" t="s">
@@ -12922,11 +12931,43 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{736F4C30-9736-4CFB-ADF5-BC9C2F0A5462}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{BA2419C9-95D6-4BD9-ADD3-F850833ECDA4}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{02C5DA5E-D3B4-4BBE-9F8A-3A9FD0A3D314}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{ECCADCD5-3D5B-4064-BF11-8CD8260C5034}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{B5AD5348-05B6-4250-A4FD-7132CFA09DBA}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{1680D33A-BB13-455F-84EE-44DE8B597F75}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{BDD80B2B-5344-444A-A3F3-92EC5E666528}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{3E5C669B-B6C2-4551-BB59-A3EB69626396}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{BF954CAA-C8FD-466A-AB65-CE12BFA69801}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{2466AE46-3740-4DEA-B26D-662C5B8D3B9F}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{3AFDE039-BA59-4CE1-83ED-78416F8E971C}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{5EA1A8F0-8BDA-4965-B5A2-87FC44B079E1}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{54E7C3A8-DB96-49CD-BE9C-4F605FC35322}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{E41D960F-8E9C-4213-B172-1E1ABE16C4E0}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{022A3CD0-8117-4C79-95D7-420290D0B475}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{3BC42B8E-5E51-4E70-9D93-5D5952BB72A4}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{49E61EF4-FB49-45FA-A587-F0789C9A4116}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{2908BA46-F66E-4147-8A21-D91E278F9470}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{A40B81B5-D170-459F-BD06-4736300B8563}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{ECB8EF1C-E9F7-463F-868F-351EA90A1B1F}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{7EBE3A33-C150-4917-97D3-304FDAE7222B}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{DA59273D-6FF9-4861-A5DD-E2B3CCD46CF5}"/>
+    <hyperlink ref="F2" r:id="rId23" xr:uid="{4A7A5DEA-D7E4-4F04-BEE6-E5439B65F815}"/>
+    <hyperlink ref="F3" r:id="rId24" xr:uid="{EB2E96DF-E1EE-415F-AF83-01581AF114D6}"/>
+    <hyperlink ref="H2" r:id="rId25" xr:uid="{973E5923-1197-49F8-8837-4E47E7F774B2}"/>
+    <hyperlink ref="H3:H13" r:id="rId26" display="भारत" xr:uid="{21CF1BB5-1759-4D9C-9E12-FC9B6EF20337}"/>
+    <hyperlink ref="H14" r:id="rId27" xr:uid="{A3AAB5CB-360A-4877-AB1B-FE23CBDAAC76}"/>
+    <hyperlink ref="H15:H17" r:id="rId28" display="Singapore" xr:uid="{F4F13671-BCDD-4054-89F8-2FC322D3549B}"/>
+    <hyperlink ref="H18" r:id="rId29" xr:uid="{48A08E36-25FB-45AF-8613-CB8A0BD468DB}"/>
+    <hyperlink ref="H19:H25" r:id="rId30" display="USA" xr:uid="{38486A27-886B-4407-A152-6B8625EB5DC9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId31"/>
+    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId33"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
ENH: gramex.cache.open(excel) supports hyperlinks. Fixes #722 (#754)
</commit_message>
<xml_diff>
--- a/tests/sales.xlsx
+++ b/tests/sales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\site\gramener.com\viz\async-gramex\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\site\gramener.com\viz\async-gramex\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B960B43A-7FA7-4EEC-906F-DBE12E69798F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4BAC76-22CE-477D-BACB-5FB8165625D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6EE3D399-FAD5-3F44-9EB5-0B167948DCE0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{6EE3D399-FAD5-3F44-9EB5-0B167948DCE0}"/>
   </bookViews>
   <sheets>
     <sheet name="sales" sheetId="1" r:id="rId1"/>
@@ -4032,10 +4032,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4058,14 +4066,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -4433,9 +4444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5832FD-D67F-1D4C-95D0-0EB623A26DB3}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12277,13 +12286,13 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I2" t="s">
@@ -12309,13 +12318,13 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I3" t="s">
@@ -12341,13 +12350,13 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I4" t="s">
@@ -12373,13 +12382,13 @@
       <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I5" t="s">
@@ -12405,13 +12414,13 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I6" t="s">
@@ -12437,13 +12446,13 @@
       <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I7" t="s">
@@ -12469,13 +12478,13 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I8" t="s">
@@ -12501,13 +12510,13 @@
       <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F9" t="s">
         <v>37</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I9" t="s">
@@ -12533,13 +12542,13 @@
       <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I10" t="s">
@@ -12565,13 +12574,13 @@
       <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I11" t="s">
@@ -12585,13 +12594,13 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F12" t="s">
         <v>43</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I12" t="s">
@@ -12611,13 +12620,13 @@
       <c r="D13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F13" t="s">
         <v>45</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I13" t="s">
@@ -12637,13 +12646,13 @@
       <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F14" t="s">
         <v>47</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I14" t="s">
@@ -12663,13 +12672,13 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F15" t="s">
         <v>49</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I15" t="s">
@@ -12689,13 +12698,13 @@
       <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F16" t="s">
         <v>51</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I16" t="s">
@@ -12715,13 +12724,13 @@
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F17" t="s">
         <v>53</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I17" t="s">
@@ -12741,13 +12750,13 @@
       <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F18" t="s">
         <v>55</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I18" t="s">
@@ -12767,13 +12776,13 @@
       <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F19" t="s">
         <v>57</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I19" t="s">
@@ -12793,13 +12802,13 @@
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F20" t="s">
         <v>59</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I20" t="s">
@@ -12819,13 +12828,13 @@
       <c r="D21" t="s">
         <v>21</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F21" t="s">
         <v>61</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I21" t="s">
@@ -12845,13 +12854,13 @@
       <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F22" t="s">
         <v>63</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I22" t="s">
@@ -12871,13 +12880,13 @@
       <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F23" t="s">
         <v>65</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I23" t="s">
@@ -12894,7 +12903,7 @@
       </c>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H24" t="s">
+      <c r="H24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I24" t="s">
@@ -12911,7 +12920,7 @@
       </c>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
+      <c r="H25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I25" t="s">
@@ -12922,11 +12931,43 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{736F4C30-9736-4CFB-ADF5-BC9C2F0A5462}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{BA2419C9-95D6-4BD9-ADD3-F850833ECDA4}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{02C5DA5E-D3B4-4BBE-9F8A-3A9FD0A3D314}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{ECCADCD5-3D5B-4064-BF11-8CD8260C5034}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{B5AD5348-05B6-4250-A4FD-7132CFA09DBA}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{1680D33A-BB13-455F-84EE-44DE8B597F75}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{BDD80B2B-5344-444A-A3F3-92EC5E666528}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{3E5C669B-B6C2-4551-BB59-A3EB69626396}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{BF954CAA-C8FD-466A-AB65-CE12BFA69801}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{2466AE46-3740-4DEA-B26D-662C5B8D3B9F}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{3AFDE039-BA59-4CE1-83ED-78416F8E971C}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{5EA1A8F0-8BDA-4965-B5A2-87FC44B079E1}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{54E7C3A8-DB96-49CD-BE9C-4F605FC35322}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{E41D960F-8E9C-4213-B172-1E1ABE16C4E0}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{022A3CD0-8117-4C79-95D7-420290D0B475}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{3BC42B8E-5E51-4E70-9D93-5D5952BB72A4}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{49E61EF4-FB49-45FA-A587-F0789C9A4116}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{2908BA46-F66E-4147-8A21-D91E278F9470}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{A40B81B5-D170-459F-BD06-4736300B8563}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{ECB8EF1C-E9F7-463F-868F-351EA90A1B1F}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{7EBE3A33-C150-4917-97D3-304FDAE7222B}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{DA59273D-6FF9-4861-A5DD-E2B3CCD46CF5}"/>
+    <hyperlink ref="F2" r:id="rId23" xr:uid="{4A7A5DEA-D7E4-4F04-BEE6-E5439B65F815}"/>
+    <hyperlink ref="F3" r:id="rId24" xr:uid="{EB2E96DF-E1EE-415F-AF83-01581AF114D6}"/>
+    <hyperlink ref="H2" r:id="rId25" xr:uid="{973E5923-1197-49F8-8837-4E47E7F774B2}"/>
+    <hyperlink ref="H3:H13" r:id="rId26" display="भारत" xr:uid="{21CF1BB5-1759-4D9C-9E12-FC9B6EF20337}"/>
+    <hyperlink ref="H14" r:id="rId27" xr:uid="{A3AAB5CB-360A-4877-AB1B-FE23CBDAAC76}"/>
+    <hyperlink ref="H15:H17" r:id="rId28" display="Singapore" xr:uid="{F4F13671-BCDD-4054-89F8-2FC322D3549B}"/>
+    <hyperlink ref="H18" r:id="rId29" xr:uid="{48A08E36-25FB-45AF-8613-CB8A0BD468DB}"/>
+    <hyperlink ref="H19:H25" r:id="rId30" display="USA" xr:uid="{38486A27-886B-4407-A152-6B8625EB5DC9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId31"/>
+    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId33"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>